<commit_message>
Custom Iowa + Louisville scenario
</commit_message>
<xml_diff>
--- a/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
+++ b/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/580bce16df9ec0bf/Documents/Navigate/CFP Simulator/Input Data/Update Elo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F976C161-963B-4107-A723-F10FBB2EF515}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE0C615B-3319-4E6E-B4BB-2383463961D9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="237">
   <si>
     <t>Week</t>
   </si>
@@ -1097,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H859"/>
+  <dimension ref="A1:H860"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A847" workbookViewId="0">
-      <selection activeCell="G860" sqref="G860"/>
+      <selection activeCell="D861" sqref="D861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20865,6 +20865,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="860" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A860">
+        <v>15</v>
+      </c>
+      <c r="B860" t="s">
+        <v>89</v>
+      </c>
+      <c r="C860" t="s">
+        <v>112</v>
+      </c>
+      <c r="E860">
+        <v>1</v>
+      </c>
+      <c r="F860">
+        <v>9</v>
+      </c>
+      <c r="G860">
+        <v>1</v>
+      </c>
+      <c r="H860">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Custom Alabama + Louisville scenario
</commit_message>
<xml_diff>
--- a/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
+++ b/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/580bce16df9ec0bf/Documents/Navigate/CFP Simulator/Input Data/Update Elo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF497BFA-A710-4C9C-8C0C-2F0C4A7F6EE3}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CC87F5-4BE5-4595-96EB-AAAA1DB58CAC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="237">
   <si>
     <t>Week</t>
   </si>
@@ -1097,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H859"/>
+  <dimension ref="A1:H860"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
-      <selection activeCell="B860" sqref="B860"/>
+    <sheetView tabSelected="1" topLeftCell="A847" workbookViewId="0">
+      <selection activeCell="A861" sqref="A861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20865,6 +20865,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="860" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A860">
+        <v>15</v>
+      </c>
+      <c r="B860" t="s">
+        <v>49</v>
+      </c>
+      <c r="C860" t="s">
+        <v>176</v>
+      </c>
+      <c r="E860">
+        <v>1</v>
+      </c>
+      <c r="F860">
+        <v>9</v>
+      </c>
+      <c r="G860">
+        <v>1</v>
+      </c>
+      <c r="H860">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Custom Louisville + OKState + Alabama + Iowa scenario
</commit_message>
<xml_diff>
--- a/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
+++ b/Input Data/Update Elo/CFB_Sch_23-24 (Completed) - Theoretical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/580bce16df9ec0bf/Documents/Navigate/CFP Simulator/Input Data/Update Elo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CC87F5-4BE5-4595-96EB-AAAA1DB58CAC}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_1C3D1EC04545D40E62355476585DCE3A8743FBDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{719F99B4-FD0E-424A-AEBE-3E1C6FC4B167}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="237">
   <si>
     <t>Week</t>
   </si>
@@ -1097,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H860"/>
+  <dimension ref="A1:H862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A847" workbookViewId="0">
-      <selection activeCell="A861" sqref="A861"/>
+    <sheetView tabSelected="1" topLeftCell="A850" workbookViewId="0">
+      <selection activeCell="D863" sqref="D863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20888,6 +20888,52 @@
         <v>0</v>
       </c>
     </row>
+    <row r="861" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A861">
+        <v>15</v>
+      </c>
+      <c r="B861" t="s">
+        <v>89</v>
+      </c>
+      <c r="C861" t="s">
+        <v>112</v>
+      </c>
+      <c r="E861">
+        <v>1</v>
+      </c>
+      <c r="F861">
+        <v>9</v>
+      </c>
+      <c r="G861">
+        <v>1</v>
+      </c>
+      <c r="H861">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="862" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A862">
+        <v>15</v>
+      </c>
+      <c r="B862" t="s">
+        <v>131</v>
+      </c>
+      <c r="C862" t="s">
+        <v>150</v>
+      </c>
+      <c r="E862">
+        <v>1</v>
+      </c>
+      <c r="F862">
+        <v>9</v>
+      </c>
+      <c r="G862">
+        <v>1</v>
+      </c>
+      <c r="H862">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>